<commit_message>
Minor bug fix before the soft launch
</commit_message>
<xml_diff>
--- a/polls/IROS20_Specials.xlsx
+++ b/polls/IROS20_Specials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF5EB82-7B47-4410-B3C0-034BF924D3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FCB50C-FA0D-47C0-87FF-F93EC29AF1D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A409DE9B-95F8-4915-A0F8-147B34139FE7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A409DE9B-95F8-4915-A0F8-147B34139FE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="116">
   <si>
     <t>Genre</t>
   </si>
@@ -329,12 +329,69 @@
   <si>
     <t xml:space="preserve">Ashish D. Deshpande is a faculty member in the Mechanical Engineering Department at the University of Texas since 2011. Dr. Deshpande received his Ph.D. degree in Mechanical Engineering from the University of Michigan, Ann Arbor, in 2007. He then completed a post-doctoral fellowship at the University of Washington in Seattle. At The University of Texas at Austin, Dr. Deshpande directs the ReNeu Robotics Lab. His work focuses on the study of human system and design of robotic systems toward the goals accelerating recovery after a neurological injury (e.g. stroke and spinal cord injury), improving the quality of lives of those living disabilities (e.g. amputation) and enhancing lives and productivity of workers, soldiers and astronauts. Specifically, his group has designed two novel exoskeletons for delivering engaging and subject-specific training for neuro-recovery of upper-body movements after stroke and spinal cord injury. Currently his group is collaborating with top clinicians around the world to combine technological advances with fundamental understanding of both healthy and affected human neuromotor system toward improving patient care. Accomplishing dexterous manipulation through the study of human hands and by making advances in robot design and control is another area of focus for Dr. Deshpande’s group. Dr. Deshpande is a co-founder of Harmonic Bionics whose mission is to improve rehabilitation outcomes for the stroke patients. Dr. Deshpande is recipient of the NSF’s prestigious CAREER Award. </t>
   </si>
+  <si>
+    <t>Real Roboticist - Michelle Johnson - Robots that Matter</t>
+  </si>
+  <si>
+    <t>Real Roboticist - Davide Scaramuzza - Drones &amp; Magic</t>
+  </si>
+  <si>
+    <t>Real Roboticist - Dennis Hong - Making People Happy</t>
+  </si>
+  <si>
+    <t>Real Roboticist - Ruzena Bajczy - Foundations</t>
+  </si>
+  <si>
+    <t>Real Roboticist - Peter Corke - Learning</t>
+  </si>
+  <si>
+    <t>3970_WV.mp4</t>
+  </si>
+  <si>
+    <t>3971_WV.mp4</t>
+  </si>
+  <si>
+    <t>3972_WV.mp4</t>
+  </si>
+  <si>
+    <t>3973_WV.mp4</t>
+  </si>
+  <si>
+    <t>3974_WV.mp4</t>
+  </si>
+  <si>
+    <t>BiR-IROS: Black in Robotics IROS 2020</t>
+  </si>
+  <si>
+    <t>BiR-IROS Launch Event</t>
+  </si>
+  <si>
+    <t>BiR Student Event</t>
+  </si>
+  <si>
+    <t>BiR Allies Engagement Event</t>
+  </si>
+  <si>
+    <t>3975_WV.mp4</t>
+  </si>
+  <si>
+    <t>3976_WV.mp4</t>
+  </si>
+  <si>
+    <t>3977_WV.mp4</t>
+  </si>
+  <si>
+    <t>Howard, Ayanna</t>
+  </si>
+  <si>
+    <t>Georgia Institute of Technology</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +460,29 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -440,7 +520,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,13 +554,24 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -802,7 +893,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -901,7 +992,7 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="16" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="5">
@@ -962,10 +1053,10 @@
       <c r="C6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="15" t="s">
         <v>74</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -989,10 +1080,10 @@
       <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>76</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -1016,10 +1107,10 @@
       <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="15" t="s">
         <v>78</v>
       </c>
       <c r="G8" s="11" t="s">
@@ -1043,10 +1134,10 @@
       <c r="C9" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="15" t="s">
         <v>80</v>
       </c>
       <c r="F9" t="s">
@@ -1073,10 +1164,10 @@
       <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>82</v>
       </c>
       <c r="F10" t="s">
@@ -1103,10 +1194,10 @@
       <c r="C11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>84</v>
       </c>
       <c r="F11" t="s">
@@ -1133,10 +1224,10 @@
       <c r="C12" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>95</v>
       </c>
       <c r="G12" s="12" t="s">
@@ -1160,10 +1251,10 @@
       <c r="C13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>86</v>
       </c>
       <c r="F13" t="s">
@@ -1175,10 +1266,10 @@
       <c r="H13" s="5">
         <v>10011</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="17"/>
+      <c r="J13" s="22"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
@@ -1192,10 +1283,10 @@
       <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>88</v>
       </c>
       <c r="G14" s="12" t="s">
@@ -1204,11 +1295,11 @@
       <c r="H14" s="5">
         <v>10012</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
@@ -1242,7 +1333,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" s="14" customFormat="1">
+    <row r="18" spans="1:14" s="13" customFormat="1" ht="15.75">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1253,8 +1344,13 @@
         <v>55</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="7"/>
+      <c r="E18" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="F18" s="1"/>
+      <c r="G18" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="H18" s="5">
         <v>10013</v>
       </c>
@@ -1262,10 +1358,10 @@
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
-      <c r="M18" s="15"/>
+      <c r="M18" s="14"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" s="14" customFormat="1">
+    <row r="19" spans="1:14" s="13" customFormat="1" ht="15.75">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1276,8 +1372,13 @@
         <v>57</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="17" t="s">
+        <v>98</v>
+      </c>
       <c r="F19" s="1"/>
+      <c r="G19" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="H19" s="5">
         <v>10014</v>
       </c>
@@ -1285,10 +1386,10 @@
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
-      <c r="M19" s="15"/>
+      <c r="M19" s="14"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" s="14" customFormat="1">
+    <row r="20" spans="1:14" s="13" customFormat="1" ht="15.75">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1299,8 +1400,13 @@
         <v>59</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="17" t="s">
+        <v>99</v>
+      </c>
       <c r="F20" s="1"/>
+      <c r="G20" s="19" t="s">
+        <v>104</v>
+      </c>
       <c r="H20" s="5">
         <v>10015</v>
       </c>
@@ -1308,10 +1414,10 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="15"/>
+      <c r="M20" s="14"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" s="14" customFormat="1">
+    <row r="21" spans="1:14" s="13" customFormat="1" ht="15.75">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1322,8 +1428,13 @@
         <v>61</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="F21" s="1"/>
+      <c r="G21" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="H21" s="5">
         <v>10016</v>
       </c>
@@ -1331,10 +1442,10 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="15"/>
+      <c r="M21" s="14"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:14" s="14" customFormat="1">
+    <row r="22" spans="1:14" s="13" customFormat="1" ht="15.75">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1345,8 +1456,13 @@
         <v>63</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="F22" s="1"/>
+      <c r="G22" s="19" t="s">
+        <v>106</v>
+      </c>
       <c r="H22" s="5">
         <v>10017</v>
       </c>
@@ -1354,19 +1470,74 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="15"/>
+      <c r="M22" s="14"/>
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="1:14">
+      <c r="E23" s="18"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" ht="15.75">
+      <c r="A24" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="20">
+        <v>10018</v>
+      </c>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" ht="15.75">
+      <c r="A25" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="20">
+        <v>10019</v>
+      </c>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" ht="15.75">
+      <c r="A26" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H26" s="20">
+        <v>10020</v>
+      </c>
       <c r="M26" s="1"/>
     </row>
   </sheetData>

</xml_diff>